<commit_message>
Lowered Training Episodes and Comments
</commit_message>
<xml_diff>
--- a/experiment_results.xlsx
+++ b/experiment_results.xlsx
@@ -742,187 +742,187 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>203.2</v>
+        <v>89.5</v>
       </c>
       <c r="B2" t="n">
-        <v>59.78762413744168</v>
+        <v>3.721558813185679</v>
       </c>
       <c r="C2" t="n">
-        <v>195.5</v>
+        <v>91.3</v>
       </c>
       <c r="D2" t="n">
-        <v>8.163945124754331</v>
+        <v>2.934280150224242</v>
       </c>
       <c r="E2" t="n">
-        <v>229.6</v>
+        <v>89.8</v>
       </c>
       <c r="F2" t="n">
-        <v>52.94563249220845</v>
+        <v>2.638181191654584</v>
       </c>
       <c r="G2" t="n">
-        <v>226.2</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="H2" t="n">
-        <v>64.70208651967879</v>
+        <v>3.006659275674582</v>
       </c>
       <c r="I2" t="n">
-        <v>244.1</v>
+        <v>90.59999999999999</v>
       </c>
       <c r="J2" t="n">
-        <v>61.0990179953819</v>
+        <v>3.611094017053557</v>
       </c>
       <c r="K2" t="n">
-        <v>223.3</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="L2" t="n">
-        <v>27.57553263311518</v>
+        <v>3.389690251335658</v>
       </c>
       <c r="M2" t="n">
-        <v>222.6</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="N2" t="n">
-        <v>29.50999830565905</v>
+        <v>2.808914381037628</v>
       </c>
       <c r="O2" t="n">
-        <v>220.2</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="P2" t="n">
-        <v>32.69495373907111</v>
+        <v>1.3</v>
       </c>
       <c r="Q2" t="n">
-        <v>203.1</v>
+        <v>92.7</v>
       </c>
       <c r="R2" t="n">
-        <v>33.92771728248159</v>
+        <v>2.865309756378881</v>
       </c>
       <c r="S2" t="n">
-        <v>225.1</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="T2" t="n">
-        <v>22.42074931843269</v>
+        <v>2.2</v>
       </c>
       <c r="U2" t="n">
-        <v>224.5</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="V2" t="n">
-        <v>32.32413958638342</v>
+        <v>3.072458299147443</v>
       </c>
       <c r="W2" t="n">
-        <v>226.5</v>
+        <v>95</v>
       </c>
       <c r="X2" t="n">
-        <v>16.28035626145816</v>
+        <v>4</v>
       </c>
       <c r="Y2" t="n">
-        <v>234.4</v>
+        <v>95.2</v>
       </c>
       <c r="Z2" t="n">
-        <v>20.48511654836262</v>
+        <v>3.218695387886216</v>
       </c>
       <c r="AA2" t="n">
-        <v>217.8</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="AB2" t="n">
-        <v>26.14880494401226</v>
+        <v>4.223742416388575</v>
       </c>
       <c r="AC2" t="n">
-        <v>218.6</v>
+        <v>95</v>
       </c>
       <c r="AD2" t="n">
-        <v>30.75776324767456</v>
+        <v>2.607680962081059</v>
       </c>
       <c r="AE2" t="n">
-        <v>201.8</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="AF2" t="n">
-        <v>27.44011661782799</v>
+        <v>5.467174773134658</v>
       </c>
       <c r="AG2" t="n">
-        <v>227.3</v>
+        <v>95.90000000000001</v>
       </c>
       <c r="AH2" t="n">
-        <v>26.44257929930437</v>
+        <v>3.726929030716844</v>
       </c>
       <c r="AI2" t="n">
-        <v>218.1</v>
+        <v>97</v>
       </c>
       <c r="AJ2" t="n">
-        <v>23.30429145028872</v>
+        <v>2.863564212655271</v>
       </c>
       <c r="AK2" t="n">
-        <v>226.6</v>
+        <v>97.40000000000001</v>
       </c>
       <c r="AL2" t="n">
-        <v>28.35207223467096</v>
+        <v>2.244994432064364</v>
       </c>
       <c r="AM2" t="n">
-        <v>217.5</v>
+        <v>97.8</v>
       </c>
       <c r="AN2" t="n">
-        <v>27.14129694764051</v>
+        <v>4.1182520563948</v>
       </c>
       <c r="AO2" t="n">
-        <v>202.3</v>
+        <v>98.8</v>
       </c>
       <c r="AP2" t="n">
-        <v>30.24251973629181</v>
+        <v>2.675817632051931</v>
       </c>
       <c r="AQ2" t="n">
-        <v>219.1</v>
+        <v>98</v>
       </c>
       <c r="AR2" t="n">
-        <v>22.44303900990238</v>
+        <v>3.16227766016838</v>
       </c>
       <c r="AS2" t="n">
-        <v>233.7</v>
+        <v>95.7</v>
       </c>
       <c r="AT2" t="n">
-        <v>21.37311395187889</v>
+        <v>2.491987158875422</v>
       </c>
       <c r="AU2" t="n">
-        <v>213.7</v>
+        <v>96.8</v>
       </c>
       <c r="AV2" t="n">
-        <v>21.1094765449075</v>
+        <v>3.059411708155671</v>
       </c>
       <c r="AW2" t="n">
-        <v>203.6</v>
+        <v>95.7</v>
       </c>
       <c r="AX2" t="n">
-        <v>40.05046816205773</v>
+        <v>4.670117771534247</v>
       </c>
       <c r="AY2" t="n">
-        <v>236.4</v>
+        <v>94.5</v>
       </c>
       <c r="AZ2" t="n">
-        <v>39.17703408886385</v>
+        <v>3.640054944640259</v>
       </c>
       <c r="BA2" t="n">
-        <v>230.5</v>
+        <v>94.90000000000001</v>
       </c>
       <c r="BB2" t="n">
-        <v>42.01963826593466</v>
+        <v>4.253234063627347</v>
       </c>
       <c r="BC2" t="n">
-        <v>202.5</v>
+        <v>93.2</v>
       </c>
       <c r="BD2" t="n">
-        <v>23.21745033374681</v>
+        <v>3.841874542459709</v>
       </c>
       <c r="BE2" t="n">
-        <v>208.1</v>
+        <v>93.3</v>
       </c>
       <c r="BF2" t="n">
-        <v>17.3692256591939</v>
+        <v>5.080354318352215</v>
       </c>
       <c r="BG2" t="n">
-        <v>204.1</v>
+        <v>92</v>
       </c>
       <c r="BH2" t="n">
-        <v>25.41436601609413</v>
+        <v>4.604345773288535</v>
       </c>
       <c r="BI2" t="n">
-        <v>6560.000000000001</v>
+        <v>2832.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>